<commit_message>
adding rest assured dependancy
</commit_message>
<xml_diff>
--- a/src/test/java/testData/testData_1.xlsx
+++ b/src/test/java/testData/testData_1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikhil\Automation\UI_Automation_3\AutomationFramework\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49161A88-A40D-4BCF-8D6F-93A98B59C30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ADB224-175A-48C4-A3FE-50C57542CE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserDatails" sheetId="1" r:id="rId1"/>
+    <sheet name="UserCredentials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Test_Case_Name</t>
   </si>
@@ -123,10 +124,16 @@
     <t>Result</t>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>DataProviderWithExcel_001</t>
+  </si>
+  <si>
+    <t>DataProviderWithExcel_002</t>
+  </si>
+  <si>
     <t>Fail</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -134,7 +141,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,13 +157,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -172,9 +193,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -458,12 +480,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" customWidth="true" width="20.85546875"/>
+    <col min="2" max="2" customWidth="true" width="15.140625"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="11.0"/>
   </cols>
   <sheetData>
@@ -552,7 +577,7 @@
         <v>29</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -605,4 +630,62 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F6506A-3403-4A1B-B0A1-27833A3F35FD}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="28.140625"/>
+    <col min="2" max="2" customWidth="true" width="17.7109375"/>
+    <col min="3" max="3" customWidth="true" width="17.5703125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{AE993E09-F428-4193-9E64-4BF4FBCF1E9B}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{1D188B35-D90A-43C1-A3B7-0E9C8FB60618}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>